<commit_message>
Newer data and PMGWeb to upload Done
</commit_message>
<xml_diff>
--- a/DMSGPT/src/mazdaNelspruit/cars.xlsx
+++ b/DMSGPT/src/mazdaNelspruit/cars.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
   <si>
     <t>Vehicle_Name</t>
   </si>
@@ -35,19 +35,19 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Nissan NP300 2.5 TDi Hi-Rider Single-Cab</t>
-  </si>
-  <si>
-    <t>UG5413</t>
+    <t>Toyota Hilux 2.8GD-6 Double Cab 4x4 Legend 50 Auto</t>
+  </si>
+  <si>
+    <t>UG5438</t>
   </si>
   <si>
     <t>Used</t>
   </si>
   <si>
-    <t>256 000 Km</t>
-  </si>
-  <si>
-    <t>R 139 900</t>
+    <t>75 000 Km</t>
+  </si>
+  <si>
+    <t>R 619 900</t>
   </si>
   <si>
     <t>Mazda CX-5 2.0 Dynamic Auto</t>
@@ -185,18 +185,6 @@
     <t>R 159 900</t>
   </si>
   <si>
-    <t>Toyota Fortuner 2.5 D-4D Raised Body Auto</t>
-  </si>
-  <si>
-    <t>UG5380</t>
-  </si>
-  <si>
-    <t>266 100 Km</t>
-  </si>
-  <si>
-    <t>R 289 000</t>
-  </si>
-  <si>
     <t>Opel Adam 1.0T Jam</t>
   </si>
   <si>
@@ -219,18 +207,6 @@
   </si>
   <si>
     <t>R 349 900</t>
-  </si>
-  <si>
-    <t>Ford Ranger 3.2 TDCi XLT 4x4 Auto Double-Cab</t>
-  </si>
-  <si>
-    <t>UG5359</t>
-  </si>
-  <si>
-    <t>134 000 Km</t>
-  </si>
-  <si>
-    <t>R 249 900</t>
   </si>
   <si>
     <t>Volkswagen T-Roc 2.0 TSI Design 4Motion Auto</t>
@@ -335,7 +311,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -369,7 +345,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>1.0133103E7</v>
+        <v>1.0141375E7</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -378,7 +354,7 @@
         <v>9</v>
       </c>
       <c r="E2" t="n">
-        <v>2009.0</v>
+        <v>2020.0</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -668,7 +644,7 @@
         <v>57</v>
       </c>
       <c r="B15" t="n">
-        <v>1.0014875E7</v>
+        <v>9991649.0</v>
       </c>
       <c r="C15" t="s">
         <v>58</v>
@@ -677,7 +653,7 @@
         <v>9</v>
       </c>
       <c r="E15" t="n">
-        <v>2016.0</v>
+        <v>2018.0</v>
       </c>
       <c r="F15" t="s">
         <v>59</v>
@@ -691,7 +667,7 @@
         <v>61</v>
       </c>
       <c r="B16" t="n">
-        <v>9991649.0</v>
+        <v>9986675.0</v>
       </c>
       <c r="C16" t="s">
         <v>62</v>
@@ -700,7 +676,7 @@
         <v>9</v>
       </c>
       <c r="E16" t="n">
-        <v>2018.0</v>
+        <v>2021.0</v>
       </c>
       <c r="F16" t="s">
         <v>63</v>
@@ -714,7 +690,7 @@
         <v>65</v>
       </c>
       <c r="B17" t="n">
-        <v>9986675.0</v>
+        <v>9968789.0</v>
       </c>
       <c r="C17" t="s">
         <v>66</v>
@@ -729,53 +705,53 @@
         <v>67</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="n">
+        <v>9937815.0</v>
+      </c>
+      <c r="C18" t="s">
         <v>69</v>
       </c>
-      <c r="B18" t="n">
-        <v>9984385.0</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2023.0</v>
+      </c>
+      <c r="F18" t="s">
         <v>70</v>
       </c>
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" t="n">
-        <v>2014.0</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>71</v>
-      </c>
-      <c r="G18" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="n">
+        <v>9919374.0</v>
+      </c>
+      <c r="C19" t="s">
         <v>73</v>
       </c>
-      <c r="B19" t="n">
-        <v>9968789.0</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2013.0</v>
+      </c>
+      <c r="F19" t="s">
         <v>74</v>
       </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" t="n">
-        <v>2021.0</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>75</v>
-      </c>
-      <c r="G19" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="20">
@@ -783,7 +759,7 @@
         <v>76</v>
       </c>
       <c r="B20" t="n">
-        <v>9937815.0</v>
+        <v>9902989.0</v>
       </c>
       <c r="C20" t="s">
         <v>77</v>
@@ -792,7 +768,7 @@
         <v>9</v>
       </c>
       <c r="E20" t="n">
-        <v>2023.0</v>
+        <v>2015.0</v>
       </c>
       <c r="F20" t="s">
         <v>78</v>
@@ -803,71 +779,25 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="n">
+        <v>9894412.0</v>
+      </c>
+      <c r="C21" t="s">
         <v>80</v>
       </c>
-      <c r="B21" t="n">
-        <v>9919374.0</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2024.0</v>
+      </c>
+      <c r="F21" t="s">
         <v>81</v>
       </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" t="n">
-        <v>2013.0</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>82</v>
-      </c>
-      <c r="G21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" t="n">
-        <v>9902989.0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" t="n">
-        <v>2015.0</v>
-      </c>
-      <c r="F22" t="s">
-        <v>86</v>
-      </c>
-      <c r="G22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" t="n">
-        <v>9894412.0</v>
-      </c>
-      <c r="C23" t="s">
-        <v>88</v>
-      </c>
-      <c r="D23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" t="n">
-        <v>2024.0</v>
-      </c>
-      <c r="F23" t="s">
-        <v>89</v>
-      </c>
-      <c r="G23" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>